<commit_message>
can upload to s3
</commit_message>
<xml_diff>
--- a/docs/src/TIN_検査推移.xlsx
+++ b/docs/src/TIN_検査推移.xlsx
@@ -117,8 +117,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="33">
+  <cellStyleXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -157,7 +165,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="56" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="33">
+  <cellStyles count="41">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
@@ -174,6 +182,10 @@
     <cellStyle name="ハイパーリンク" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
@@ -191,6 +203,10 @@
     <cellStyle name="表示済みのハイパーリンク" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="40" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -519,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K87"/>
+  <dimension ref="A1:L87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="K61" sqref="K61:K87"/>
+    <sheetView tabSelected="1" topLeftCell="B46" workbookViewId="0">
+      <selection activeCell="L61" sqref="L61:L87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -570,8 +586,8 @@
         <v>1.1764705882352942</v>
       </c>
       <c r="H2" t="str">
-        <f>"["&amp;C2&amp;", "&amp;G2&amp;"]"</f>
-        <v>[-260, 1.17647058823529]</v>
+        <f>"["&amp;G2&amp;", "&amp;C2&amp;"]"</f>
+        <v>[1.17647058823529, -260]</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -594,8 +610,8 @@
         <v>1.1904761904761905</v>
       </c>
       <c r="H3" t="str">
-        <f t="shared" ref="H3:H39" si="3">"["&amp;C3&amp;", "&amp;G3&amp;"]"</f>
-        <v>[-259, 1.19047619047619]</v>
+        <f t="shared" ref="H3:H39" si="3">"["&amp;G3&amp;", "&amp;C3&amp;"]"</f>
+        <v>[1.19047619047619, -259]</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -619,7 +635,7 @@
       </c>
       <c r="H4" t="str">
         <f t="shared" si="3"/>
-        <v>[-258, 1.14942528735632]</v>
+        <v>[1.14942528735632, -258]</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -643,7 +659,7 @@
       </c>
       <c r="H5" t="str">
         <f t="shared" si="3"/>
-        <v>[-256, 1.11111111111111]</v>
+        <v>[1.11111111111111, -256]</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -667,7 +683,7 @@
       </c>
       <c r="H6" t="str">
         <f t="shared" si="3"/>
-        <v>[-250, 1.19047619047619]</v>
+        <v>[1.19047619047619, -250]</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -691,7 +707,7 @@
       </c>
       <c r="H7" t="str">
         <f t="shared" si="3"/>
-        <v>[-246, 1.17647058823529]</v>
+        <v>[1.17647058823529, -246]</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -715,7 +731,7 @@
       </c>
       <c r="H8" t="str">
         <f t="shared" si="3"/>
-        <v>[-236, 1.13636363636364]</v>
+        <v>[1.13636363636364, -236]</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -739,7 +755,7 @@
       </c>
       <c r="H9" t="str">
         <f t="shared" si="3"/>
-        <v>[-215, 1.11111111111111]</v>
+        <v>[1.11111111111111, -215]</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -763,7 +779,7 @@
       </c>
       <c r="H10" t="str">
         <f t="shared" si="3"/>
-        <v>[-196, 1.04166666666667]</v>
+        <v>[1.04166666666667, -196]</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -787,7 +803,7 @@
       </c>
       <c r="H11" t="str">
         <f t="shared" si="3"/>
-        <v>[-187, 0.970873786407767]</v>
+        <v>[0.970873786407767, -187]</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -811,7 +827,7 @@
       </c>
       <c r="H12" t="str">
         <f t="shared" si="3"/>
-        <v>[-160, 1.11111111111111]</v>
+        <v>[1.11111111111111, -160]</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -835,7 +851,7 @@
       </c>
       <c r="H13" t="str">
         <f t="shared" si="3"/>
-        <v>[-132, 1.04166666666667]</v>
+        <v>[1.04166666666667, -132]</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -859,7 +875,7 @@
       </c>
       <c r="H14" t="str">
         <f t="shared" si="3"/>
-        <v>[-83, 1.12359550561798]</v>
+        <v>[1.12359550561798, -83]</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -883,7 +899,7 @@
       </c>
       <c r="H15" t="str">
         <f t="shared" si="3"/>
-        <v>[-27, 0.65359477124183]</v>
+        <v>[0.65359477124183, -27]</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -907,10 +923,10 @@
       </c>
       <c r="H16" t="str">
         <f t="shared" si="3"/>
-        <v>[-5, 0.526315789473684]</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11">
+        <v>[0.526315789473684, -5]</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" s="1">
         <v>42608</v>
       </c>
@@ -931,7 +947,7 @@
       </c>
       <c r="H17" t="str">
         <f t="shared" si="3"/>
-        <v>[-4, 0.5]</v>
+        <v>[0.5, -4]</v>
       </c>
       <c r="J17">
         <v>22.9</v>
@@ -939,8 +955,12 @@
       <c r="K17">
         <v>5695</v>
       </c>
-    </row>
-    <row r="18" spans="1:11">
+      <c r="L17">
+        <f>K17/100</f>
+        <v>56.95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" s="1">
         <v>42612</v>
       </c>
@@ -961,7 +981,7 @@
       </c>
       <c r="H18" t="str">
         <f t="shared" si="3"/>
-        <v>[0, 0.492610837438424]</v>
+        <v>[0.492610837438424, 0]</v>
       </c>
       <c r="J18">
         <v>20.6</v>
@@ -969,8 +989,12 @@
       <c r="K18">
         <v>5519</v>
       </c>
-    </row>
-    <row r="19" spans="1:11">
+      <c r="L18">
+        <f t="shared" ref="L18:L43" si="5">K18/100</f>
+        <v>55.19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" s="2">
         <v>42614</v>
       </c>
@@ -979,7 +1003,7 @@
         <v>262</v>
       </c>
       <c r="C19">
-        <f t="shared" ref="C19:C43" si="5">B19-$B$18</f>
+        <f t="shared" ref="C19:C43" si="6">B19-$B$18</f>
         <v>2</v>
       </c>
       <c r="E19">
@@ -991,10 +1015,10 @@
       </c>
       <c r="H19" t="str">
         <f t="shared" si="3"/>
-        <v>[2, 0.492610837438424]</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
+        <v>[0.492610837438424, 2]</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" s="2">
         <v>42616</v>
       </c>
@@ -1003,7 +1027,7 @@
         <v>264</v>
       </c>
       <c r="C20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="E20">
@@ -1015,19 +1039,19 @@
       </c>
       <c r="H20" t="str">
         <f t="shared" si="3"/>
-        <v>[4, 0.50761421319797]</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11">
+        <v>[0.50761421319797, 4]</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" s="2">
         <v>42618</v>
       </c>
       <c r="B21">
-        <f t="shared" ref="B21:B27" si="6">A21-$A$2</f>
+        <f t="shared" ref="B21:B27" si="7">A21-$A$2</f>
         <v>266</v>
       </c>
       <c r="C21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="E21">
@@ -1039,19 +1063,19 @@
       </c>
       <c r="H21" t="str">
         <f t="shared" si="3"/>
-        <v>[6, 0.50251256281407]</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
+        <v>[0.50251256281407, 6]</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22" s="2">
         <v>42620</v>
       </c>
       <c r="B22">
+        <f t="shared" si="7"/>
+        <v>268</v>
+      </c>
+      <c r="C22">
         <f t="shared" si="6"/>
-        <v>268</v>
-      </c>
-      <c r="C22">
-        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="E22">
@@ -1063,19 +1087,19 @@
       </c>
       <c r="H22" t="str">
         <f t="shared" si="3"/>
-        <v>[8, 0.510204081632653]</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11">
+        <v>[0.510204081632653, 8]</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" s="2">
         <v>42622</v>
       </c>
       <c r="B23">
+        <f t="shared" si="7"/>
+        <v>270</v>
+      </c>
+      <c r="C23">
         <f t="shared" si="6"/>
-        <v>270</v>
-      </c>
-      <c r="C23">
-        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="E23">
@@ -1087,7 +1111,7 @@
       </c>
       <c r="H23" t="str">
         <f t="shared" si="3"/>
-        <v>[10, 0.526315789473684]</v>
+        <v>[0.526315789473684, 10]</v>
       </c>
       <c r="J23">
         <v>4.9000000000000004</v>
@@ -1095,17 +1119,21 @@
       <c r="K23">
         <v>1807</v>
       </c>
-    </row>
-    <row r="24" spans="1:11">
+      <c r="L23">
+        <f t="shared" si="5"/>
+        <v>18.07</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24" s="2">
         <v>42625</v>
       </c>
       <c r="B24">
+        <f t="shared" si="7"/>
+        <v>273</v>
+      </c>
+      <c r="C24">
         <f t="shared" si="6"/>
-        <v>273</v>
-      </c>
-      <c r="C24">
-        <f t="shared" si="5"/>
         <v>13</v>
       </c>
       <c r="E24">
@@ -1117,19 +1145,19 @@
       </c>
       <c r="H24" t="str">
         <f t="shared" si="3"/>
-        <v>[13, 0.555555555555556]</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11">
+        <v>[0.555555555555556, 13]</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25" s="2">
         <v>42627</v>
       </c>
       <c r="B25">
+        <f t="shared" si="7"/>
+        <v>275</v>
+      </c>
+      <c r="C25">
         <f t="shared" si="6"/>
-        <v>275</v>
-      </c>
-      <c r="C25">
-        <f t="shared" si="5"/>
         <v>15</v>
       </c>
       <c r="E25">
@@ -1141,22 +1169,26 @@
       </c>
       <c r="H25" t="str">
         <f t="shared" si="3"/>
-        <v>[15, 0.537634408602151]</v>
+        <v>[0.537634408602151, 15]</v>
       </c>
       <c r="K25">
         <v>1129</v>
       </c>
-    </row>
-    <row r="26" spans="1:11">
+      <c r="L25">
+        <f t="shared" si="5"/>
+        <v>11.29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
       <c r="A26" s="2">
         <v>42628</v>
       </c>
       <c r="B26">
+        <f t="shared" si="7"/>
+        <v>276</v>
+      </c>
+      <c r="C26">
         <f t="shared" si="6"/>
-        <v>276</v>
-      </c>
-      <c r="C26">
-        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="E26">
@@ -1168,19 +1200,19 @@
       </c>
       <c r="H26" t="str">
         <f t="shared" si="3"/>
-        <v>[16, 0.518134715025907]</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
+        <v>[0.518134715025907, 16]</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
       <c r="A27" s="2">
         <v>42630</v>
       </c>
       <c r="B27">
+        <f t="shared" si="7"/>
+        <v>278</v>
+      </c>
+      <c r="C27">
         <f t="shared" si="6"/>
-        <v>278</v>
-      </c>
-      <c r="C27">
-        <f t="shared" si="5"/>
         <v>18</v>
       </c>
       <c r="E27">
@@ -1192,19 +1224,19 @@
       </c>
       <c r="H27" t="str">
         <f t="shared" si="3"/>
-        <v>[18, 0.561797752808989]</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11">
+        <v>[0.561797752808989, 18]</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
       <c r="A28" s="2">
         <v>42633</v>
       </c>
       <c r="B28">
-        <f t="shared" ref="B28:B43" si="7">A28-$A$2</f>
+        <f t="shared" ref="B28:B43" si="8">A28-$A$2</f>
         <v>281</v>
       </c>
       <c r="C28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>21</v>
       </c>
       <c r="E28">
@@ -1216,7 +1248,7 @@
       </c>
       <c r="H28" t="str">
         <f t="shared" si="3"/>
-        <v>[21, 0.625]</v>
+        <v>[0.625, 21]</v>
       </c>
       <c r="J28">
         <v>4.5999999999999996</v>
@@ -1224,17 +1256,21 @@
       <c r="K28">
         <v>744</v>
       </c>
-    </row>
-    <row r="29" spans="1:11">
+      <c r="L28">
+        <f t="shared" si="5"/>
+        <v>7.44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
       <c r="A29" s="2">
         <v>42636</v>
       </c>
       <c r="B29">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>284</v>
       </c>
       <c r="C29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>24</v>
       </c>
       <c r="E29">
@@ -1246,7 +1282,7 @@
       </c>
       <c r="H29" t="str">
         <f t="shared" si="3"/>
-        <v>[24, 0.680272108843537]</v>
+        <v>[0.680272108843537, 24]</v>
       </c>
       <c r="J29">
         <v>2.9</v>
@@ -1254,17 +1290,21 @@
       <c r="K29">
         <v>52</v>
       </c>
-    </row>
-    <row r="30" spans="1:11">
+      <c r="L29">
+        <f t="shared" si="5"/>
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
       <c r="A30" s="2">
         <v>42639</v>
       </c>
       <c r="B30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>287</v>
       </c>
       <c r="C30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>27</v>
       </c>
       <c r="E30">
@@ -1276,7 +1316,7 @@
       </c>
       <c r="H30" t="str">
         <f t="shared" si="3"/>
-        <v>[27, 0.680272108843537]</v>
+        <v>[0.680272108843537, 27]</v>
       </c>
       <c r="J30">
         <v>5.6</v>
@@ -1284,17 +1324,21 @@
       <c r="K30">
         <v>67</v>
       </c>
-    </row>
-    <row r="31" spans="1:11">
+      <c r="L30">
+        <f t="shared" si="5"/>
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
       <c r="A31" s="2">
         <v>42641</v>
       </c>
       <c r="B31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>289</v>
       </c>
       <c r="C31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>29</v>
       </c>
       <c r="E31">
@@ -1306,19 +1350,19 @@
       </c>
       <c r="H31" t="str">
         <f t="shared" si="3"/>
-        <v>[29, 0.689655172413793]</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11">
+        <v>[0.689655172413793, 29]</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
       <c r="A32" s="2">
         <v>42643</v>
       </c>
       <c r="B32">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>291</v>
       </c>
       <c r="C32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>31</v>
       </c>
       <c r="E32">
@@ -1330,7 +1374,7 @@
       </c>
       <c r="H32" t="str">
         <f t="shared" si="3"/>
-        <v>[31, 0.75187969924812]</v>
+        <v>[0.75187969924812, 31]</v>
       </c>
       <c r="J32">
         <v>2.9</v>
@@ -1338,17 +1382,21 @@
       <c r="K32">
         <v>75</v>
       </c>
-    </row>
-    <row r="33" spans="1:11">
+      <c r="L32">
+        <f t="shared" si="5"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
       <c r="A33" s="2">
         <v>42646</v>
       </c>
       <c r="B33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>294</v>
       </c>
       <c r="C33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>34</v>
       </c>
       <c r="E33">
@@ -1360,7 +1408,7 @@
       </c>
       <c r="H33" t="str">
         <f t="shared" si="3"/>
-        <v>[34, 0.884955752212389]</v>
+        <v>[0.884955752212389, 34]</v>
       </c>
       <c r="J33">
         <v>4</v>
@@ -1368,17 +1416,21 @@
       <c r="K33">
         <v>1400</v>
       </c>
-    </row>
-    <row r="34" spans="1:11">
+      <c r="L33">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
       <c r="A34" s="2">
         <v>42648</v>
       </c>
       <c r="B34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>296</v>
       </c>
       <c r="C34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>36</v>
       </c>
       <c r="E34">
@@ -1390,7 +1442,7 @@
       </c>
       <c r="H34" t="str">
         <f t="shared" si="3"/>
-        <v>[36, 0.892857142857143]</v>
+        <v>[0.892857142857143, 36]</v>
       </c>
       <c r="J34">
         <v>3.3</v>
@@ -1398,17 +1450,21 @@
       <c r="K34">
         <v>373</v>
       </c>
-    </row>
-    <row r="35" spans="1:11">
+      <c r="L34">
+        <f t="shared" si="5"/>
+        <v>3.73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
       <c r="A35" s="2">
         <v>42650</v>
       </c>
       <c r="B35">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>298</v>
       </c>
       <c r="C35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>38</v>
       </c>
       <c r="E35">
@@ -1420,7 +1476,7 @@
       </c>
       <c r="H35" t="str">
         <f t="shared" si="3"/>
-        <v>[38, 0.900900900900901]</v>
+        <v>[0.900900900900901, 38]</v>
       </c>
       <c r="J35">
         <v>5.9</v>
@@ -1428,17 +1484,21 @@
       <c r="K35">
         <v>394</v>
       </c>
-    </row>
-    <row r="36" spans="1:11">
+      <c r="L35">
+        <f t="shared" si="5"/>
+        <v>3.94</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
       <c r="A36" s="2">
         <v>42657</v>
       </c>
       <c r="B36">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>305</v>
       </c>
       <c r="C36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>45</v>
       </c>
       <c r="E36">
@@ -1450,7 +1510,7 @@
       </c>
       <c r="H36" t="str">
         <f t="shared" si="3"/>
-        <v>[45, 0.826446280991736]</v>
+        <v>[0.826446280991736, 45]</v>
       </c>
       <c r="J36">
         <v>7.9</v>
@@ -1458,17 +1518,21 @@
       <c r="K36">
         <v>153</v>
       </c>
-    </row>
-    <row r="37" spans="1:11">
+      <c r="L36">
+        <f t="shared" si="5"/>
+        <v>1.53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
       <c r="A37" s="2">
         <v>42671</v>
       </c>
       <c r="B37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>319</v>
       </c>
       <c r="C37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>59</v>
       </c>
       <c r="E37">
@@ -1480,7 +1544,7 @@
       </c>
       <c r="H37" t="str">
         <f t="shared" si="3"/>
-        <v>[59, 0.746268656716418]</v>
+        <v>[0.746268656716418, 59]</v>
       </c>
       <c r="J37">
         <v>11.7</v>
@@ -1488,17 +1552,21 @@
       <c r="K37">
         <v>170</v>
       </c>
-    </row>
-    <row r="38" spans="1:11">
+      <c r="L37">
+        <f t="shared" si="5"/>
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
       <c r="A38" s="2">
         <v>42674</v>
       </c>
       <c r="B38">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>322</v>
       </c>
       <c r="C38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>62</v>
       </c>
       <c r="E38">
@@ -1513,7 +1581,7 @@
       </c>
       <c r="H38" t="str">
         <f t="shared" si="3"/>
-        <v>[62, 0.840336134453782]</v>
+        <v>[0.840336134453782, 62]</v>
       </c>
       <c r="J38">
         <v>7.3</v>
@@ -1521,17 +1589,21 @@
       <c r="K38">
         <v>202</v>
       </c>
-    </row>
-    <row r="39" spans="1:11">
+      <c r="L38">
+        <f t="shared" si="5"/>
+        <v>2.02</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
       <c r="A39" s="2">
         <v>42676</v>
       </c>
       <c r="B39">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>324</v>
       </c>
       <c r="C39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>64</v>
       </c>
       <c r="E39">
@@ -1546,19 +1618,19 @@
       </c>
       <c r="H39" t="str">
         <f t="shared" si="3"/>
-        <v>[64, 0.847457627118644]</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11">
+        <v>[0.847457627118644, 64]</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
       <c r="A40" s="2">
         <v>42681</v>
       </c>
       <c r="B40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>329</v>
       </c>
       <c r="C40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>69</v>
       </c>
       <c r="J40">
@@ -1567,17 +1639,21 @@
       <c r="K40">
         <v>315</v>
       </c>
-    </row>
-    <row r="41" spans="1:11">
+      <c r="L40">
+        <f t="shared" si="5"/>
+        <v>3.15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
       <c r="A41" s="2">
         <v>42685</v>
       </c>
       <c r="B41">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>333</v>
       </c>
       <c r="C41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>73</v>
       </c>
       <c r="J41">
@@ -1586,17 +1662,21 @@
       <c r="K41">
         <v>434</v>
       </c>
-    </row>
-    <row r="42" spans="1:11">
+      <c r="L41">
+        <f t="shared" si="5"/>
+        <v>4.34</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
       <c r="A42" s="2">
         <v>42688</v>
       </c>
       <c r="B42">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>336</v>
       </c>
       <c r="C42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>76</v>
       </c>
       <c r="J42">
@@ -1605,17 +1685,21 @@
       <c r="K42">
         <v>287</v>
       </c>
-    </row>
-    <row r="43" spans="1:11">
+      <c r="L42">
+        <f t="shared" si="5"/>
+        <v>2.87</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
       <c r="A43" s="2">
         <v>42691</v>
       </c>
       <c r="B43">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>339</v>
       </c>
       <c r="C43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>79</v>
       </c>
       <c r="J43">
@@ -1624,8 +1708,12 @@
       <c r="K43">
         <v>417</v>
       </c>
-    </row>
-    <row r="46" spans="1:11">
+      <c r="L43">
+        <f t="shared" si="5"/>
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
       <c r="J46" t="str">
         <f>IF(J2="","","["&amp;$C2&amp;", "&amp;J2&amp;"]")</f>
         <v/>
@@ -1634,415 +1722,583 @@
         <f>IF(K2="","","["&amp;$C2&amp;", "&amp;K2&amp;"]")</f>
         <v/>
       </c>
-    </row>
-    <row r="47" spans="1:11">
+      <c r="L46" t="str">
+        <f>IF(L2="","","["&amp;$C2&amp;", "&amp;L2&amp;"]")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
       <c r="J47" t="str">
-        <f t="shared" ref="J47:K87" si="8">IF(J3="","","["&amp;$C3&amp;", "&amp;J3&amp;"]")</f>
+        <f t="shared" ref="J47:L87" si="9">IF(J3="","","["&amp;$C3&amp;", "&amp;J3&amp;"]")</f>
         <v/>
       </c>
       <c r="K47" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="48" spans="1:11">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L47" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
       <c r="J48" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="K48" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="49" spans="10:11">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L48" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="10:12">
       <c r="J49" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="K49" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="50" spans="10:11">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L49" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="10:12">
       <c r="J50" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="K50" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="51" spans="10:11">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L50" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="10:12">
       <c r="J51" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="K51" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="52" spans="10:11">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L51" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="10:12">
       <c r="J52" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="K52" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="53" spans="10:11">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L52" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="10:12">
       <c r="J53" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="K53" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="54" spans="10:11">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L53" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="10:12">
       <c r="J54" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="K54" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="55" spans="10:11">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L54" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="10:12">
       <c r="J55" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="K55" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="56" spans="10:11">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L55" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="10:12">
       <c r="J56" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="K56" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="57" spans="10:11">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L56" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="10:12">
       <c r="J57" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="K57" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="58" spans="10:11">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L57" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="10:12">
       <c r="J58" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="K58" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="59" spans="10:11">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L58" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="10:12">
       <c r="J59" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="K59" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="60" spans="10:11">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L59" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="10:12">
       <c r="J60" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="K60" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="61" spans="10:11">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L60" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="10:12">
       <c r="J61" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>[-4, 22.9]</v>
       </c>
       <c r="K61" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>[-4, 5695]</v>
       </c>
-    </row>
-    <row r="62" spans="10:11">
+      <c r="L61" t="str">
+        <f t="shared" si="9"/>
+        <v>[-4, 56.95]</v>
+      </c>
+    </row>
+    <row r="62" spans="10:12">
       <c r="J62" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>[0, 20.6]</v>
       </c>
       <c r="K62" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>[0, 5519]</v>
       </c>
-    </row>
-    <row r="63" spans="10:11">
+      <c r="L62" t="str">
+        <f t="shared" si="9"/>
+        <v>[0, 55.19]</v>
+      </c>
+    </row>
+    <row r="63" spans="10:12">
       <c r="J63" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="K63" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="64" spans="10:11">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L63" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="64" spans="10:12">
       <c r="J64" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="K64" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="65" spans="10:11">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L64" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="65" spans="10:12">
       <c r="J65" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="K65" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="66" spans="10:11">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L65" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="66" spans="10:12">
       <c r="J66" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="K66" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="67" spans="10:11">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L66" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="67" spans="10:12">
       <c r="J67" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>[10, 4.9]</v>
       </c>
       <c r="K67" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>[10, 1807]</v>
       </c>
-    </row>
-    <row r="68" spans="10:11">
+      <c r="L67" t="str">
+        <f t="shared" si="9"/>
+        <v>[10, 18.07]</v>
+      </c>
+    </row>
+    <row r="68" spans="10:12">
       <c r="J68" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="K68" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="69" spans="10:11">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L68" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="69" spans="10:12">
       <c r="J69" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="K69" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>[15, 1129]</v>
       </c>
-    </row>
-    <row r="70" spans="10:11">
+      <c r="L69" t="str">
+        <f t="shared" si="9"/>
+        <v>[15, 11.29]</v>
+      </c>
+    </row>
+    <row r="70" spans="10:12">
       <c r="J70" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="K70" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="71" spans="10:11">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L70" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="71" spans="10:12">
       <c r="J71" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="K71" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="72" spans="10:11">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L71" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="72" spans="10:12">
       <c r="J72" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>[21, 4.6]</v>
       </c>
       <c r="K72" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>[21, 744]</v>
       </c>
-    </row>
-    <row r="73" spans="10:11">
+      <c r="L72" t="str">
+        <f t="shared" si="9"/>
+        <v>[21, 7.44]</v>
+      </c>
+    </row>
+    <row r="73" spans="10:12">
       <c r="J73" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>[24, 2.9]</v>
       </c>
       <c r="K73" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>[24, 52]</v>
       </c>
-    </row>
-    <row r="74" spans="10:11">
+      <c r="L73" t="str">
+        <f t="shared" si="9"/>
+        <v>[24, 0.52]</v>
+      </c>
+    </row>
+    <row r="74" spans="10:12">
       <c r="J74" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>[27, 5.6]</v>
       </c>
       <c r="K74" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>[27, 67]</v>
       </c>
-    </row>
-    <row r="75" spans="10:11">
+      <c r="L74" t="str">
+        <f t="shared" si="9"/>
+        <v>[27, 0.67]</v>
+      </c>
+    </row>
+    <row r="75" spans="10:12">
       <c r="J75" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="K75" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="76" spans="10:11">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L75" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="76" spans="10:12">
       <c r="J76" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>[31, 2.9]</v>
       </c>
       <c r="K76" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>[31, 75]</v>
       </c>
-    </row>
-    <row r="77" spans="10:11">
+      <c r="L76" t="str">
+        <f t="shared" si="9"/>
+        <v>[31, 0.75]</v>
+      </c>
+    </row>
+    <row r="77" spans="10:12">
       <c r="J77" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>[34, 4]</v>
       </c>
       <c r="K77" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>[34, 1400]</v>
       </c>
-    </row>
-    <row r="78" spans="10:11">
+      <c r="L77" t="str">
+        <f t="shared" si="9"/>
+        <v>[34, 14]</v>
+      </c>
+    </row>
+    <row r="78" spans="10:12">
       <c r="J78" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>[36, 3.3]</v>
       </c>
       <c r="K78" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>[36, 373]</v>
       </c>
-    </row>
-    <row r="79" spans="10:11">
+      <c r="L78" t="str">
+        <f t="shared" si="9"/>
+        <v>[36, 3.73]</v>
+      </c>
+    </row>
+    <row r="79" spans="10:12">
       <c r="J79" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>[38, 5.9]</v>
       </c>
       <c r="K79" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>[38, 394]</v>
       </c>
-    </row>
-    <row r="80" spans="10:11">
+      <c r="L79" t="str">
+        <f t="shared" si="9"/>
+        <v>[38, 3.94]</v>
+      </c>
+    </row>
+    <row r="80" spans="10:12">
       <c r="J80" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>[45, 7.9]</v>
       </c>
       <c r="K80" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>[45, 153]</v>
       </c>
-    </row>
-    <row r="81" spans="10:11">
+      <c r="L80" t="str">
+        <f t="shared" si="9"/>
+        <v>[45, 1.53]</v>
+      </c>
+    </row>
+    <row r="81" spans="10:12">
       <c r="J81" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>[59, 11.7]</v>
       </c>
       <c r="K81" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>[59, 170]</v>
       </c>
-    </row>
-    <row r="82" spans="10:11">
+      <c r="L81" t="str">
+        <f t="shared" si="9"/>
+        <v>[59, 1.7]</v>
+      </c>
+    </row>
+    <row r="82" spans="10:12">
       <c r="J82" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>[62, 7.3]</v>
       </c>
       <c r="K82" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>[62, 202]</v>
       </c>
-    </row>
-    <row r="83" spans="10:11">
+      <c r="L82" t="str">
+        <f t="shared" si="9"/>
+        <v>[62, 2.02]</v>
+      </c>
+    </row>
+    <row r="83" spans="10:12">
       <c r="J83" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="K83" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="84" spans="10:11">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L83" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="84" spans="10:12">
       <c r="J84" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>[69, 1.4]</v>
       </c>
       <c r="K84" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>[69, 315]</v>
       </c>
-    </row>
-    <row r="85" spans="10:11">
+      <c r="L84" t="str">
+        <f t="shared" si="9"/>
+        <v>[69, 3.15]</v>
+      </c>
+    </row>
+    <row r="85" spans="10:12">
       <c r="J85" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>[73, 3.1]</v>
       </c>
       <c r="K85" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>[73, 434]</v>
       </c>
-    </row>
-    <row r="86" spans="10:11">
+      <c r="L85" t="str">
+        <f t="shared" si="9"/>
+        <v>[73, 4.34]</v>
+      </c>
+    </row>
+    <row r="86" spans="10:12">
       <c r="J86" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>[76, 2.7]</v>
       </c>
       <c r="K86" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>[76, 287]</v>
       </c>
-    </row>
-    <row r="87" spans="10:11">
+      <c r="L86" t="str">
+        <f t="shared" si="9"/>
+        <v>[76, 2.87]</v>
+      </c>
+    </row>
+    <row r="87" spans="10:12">
       <c r="J87" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>[79, 4]</v>
       </c>
       <c r="K87" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>[79, 417]</v>
+      </c>
+      <c r="L87" t="str">
+        <f t="shared" si="9"/>
+        <v>[79, 4.17]</v>
       </c>
     </row>
   </sheetData>

</xml_diff>